<commit_message>
Modifications to the UI
</commit_message>
<xml_diff>
--- a/Points/Points.xlsx
+++ b/Points/Points.xlsx
@@ -412,10 +412,10 @@
   <sheetData>
     <row r="1" ht="91.8" customHeight="1">
       <c r="A1" s="1" t="n">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B1" s="1" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>